<commit_message>
updated bug report and session notes
</commit_message>
<xml_diff>
--- a/Bug_Report.xlsx
+++ b/Bug_Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwang\OneDrive\Desktop\MCGILL\FALL 2024\ECSE 429\Project\Part1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwang\OneDrive\Desktop\MCGILL\FALL 2024\ECSE 429\Project\Part1\GitHub\ECSE429_Project_PartA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90404B8F-66E9-4A39-97FD-2C5C1E13D818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A36259-1639-4246-A5FD-ACE4F34F6AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{19A62233-E936-4153-8FE9-C2F93DCC36CA}"/>
   </bookViews>
@@ -164,9 +164,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -174,6 +171,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -513,7 +513,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,13 +526,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -552,7 +552,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="132" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -569,24 +569,24 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -595,22 +595,22 @@
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>

</xml_diff>